<commit_message>
finish hive task4 with screenshots
</commit_message>
<xml_diff>
--- a/hive/task4/report.xlsx
+++ b/hive/task4/report.xlsx
@@ -19,43 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t>partitioning/bucketing</t>
-  </si>
-  <si>
-    <t>raw</t>
-  </si>
-  <si>
-    <t>27 s 420 ms</t>
-  </si>
-  <si>
-    <t>193s 802ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raw with tez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">partitioning/bucketing with tez </t>
-  </si>
-  <si>
-    <t>raw with vectorization</t>
-  </si>
-  <si>
-    <t>partitioning/bucketing with vectorization</t>
-  </si>
-  <si>
-    <t>orc format with vectorization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">orc format with tez </t>
-  </si>
-  <si>
-    <t>orc format</t>
-  </si>
-  <si>
-    <t>завис</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>firstQuery</t>
   </si>
@@ -63,13 +27,67 @@
     <t>secondQuery</t>
   </si>
   <si>
-    <t>98s 90ms</t>
-  </si>
-  <si>
-    <t>104s 20ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~147s </t>
+    <t>188.52 (844.017)s</t>
+  </si>
+  <si>
+    <t>150.16 (866.76)s</t>
+  </si>
+  <si>
+    <t>285.66 (1868.34)s</t>
+  </si>
+  <si>
+    <t>179.75 (2398.44)s</t>
+  </si>
+  <si>
+    <t>44.56 (96.94)s</t>
+  </si>
+  <si>
+    <t>95.29 (176.54)</t>
+  </si>
+  <si>
+    <t>44.38 (73.64)s</t>
+  </si>
+  <si>
+    <t>89.76 (172.65)s</t>
+  </si>
+  <si>
+    <t>34.96 (62.3)s</t>
+  </si>
+  <si>
+    <t>89.7 (166.7)s</t>
+  </si>
+  <si>
+    <t>26.86 (60.9)s</t>
+  </si>
+  <si>
+    <t>78.56 (155.76)s</t>
+  </si>
+  <si>
+    <t>partitioned/bucketing, rc fromat, indexes</t>
+  </si>
+  <si>
+    <t>48.76 (102.67)s</t>
+  </si>
+  <si>
+    <t>36.7 (177.5)</t>
+  </si>
+  <si>
+    <t>mr, raw</t>
+  </si>
+  <si>
+    <t>mr, partitioning/bucketing</t>
+  </si>
+  <si>
+    <t>mr, rc format</t>
+  </si>
+  <si>
+    <t>tez, partitioning/bucketing</t>
+  </si>
+  <si>
+    <t>tez, rc format</t>
+  </si>
+  <si>
+    <t>vectorization, rc format</t>
   </si>
 </sst>
 </file>
@@ -93,7 +111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -119,19 +137,6 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -162,9 +167,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,99 +450,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
     <col min="6" max="6" width="28.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" customWidth="1"/>
-    <col min="9" max="9" width="38.140625" customWidth="1"/>
-    <col min="10" max="10" width="33.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="38.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="37.42578125" customWidth="1"/>
+    <col min="12" max="12" width="28.28515625" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
+      <c r="H3" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
   </sheetData>

</xml_diff>